<commit_message>
Missing 2nd sheet in input file assumes no exceptions instead of throwing an error
</commit_message>
<xml_diff>
--- a/examples/by-subject_in.xlsx
+++ b/examples/by-subject_in.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subbyte\Projects\EduGroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subbyte\Projects\EduGroup\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888E4871-D3DD-4F3D-A547-EA6F6D2DCEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0283591-490A-4E79-9074-7FE108A06EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{ED073955-356C-4706-AC64-2210F1B9B509}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="16200" windowHeight="9983" xr2:uid="{ED073955-356C-4706-AC64-2210F1B9B509}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -410,7 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6300F5D1-9F9F-4335-8DC5-6E37DF19D597}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -463,22 +462,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0164F10-2C89-4DAA-A99E-3D1397925DC3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.46484375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>